<commit_message>
Project propertyEnumCast is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/propertyEnumCast/propertyEnumCast.xlsx
+++ b/DESIGN/rules/propertyEnumCast/propertyEnumCast.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ekosolapova/work/bugs/"/>
     </mc:Choice>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Spreadsheet SpreadsheetResult mySpr()</t>
   </si>
@@ -57,12 +57,22 @@
   </si>
   <si>
     <t>=$properties.state.toString()</t>
+  </si>
+  <si>
+    <t>properties</t>
+  </si>
+  <si>
+    <t>state</t>
+  </si>
+  <si>
+    <t>AK,AS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -92,9 +102,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6367C266-F6E6-5645-B987-7780F10EA9D9}">
-  <dimension ref="D8:E11"/>
+  <dimension ref="D8:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
@@ -418,35 +437,60 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="8" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>0</v>
       </c>
+      <c r="E8" s="0"/>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
+      <c r="D9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D10" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" s="0" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D10" t="s">
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D11" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D11" t="s">
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12">
+      <c r="D12" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="F12" s="10"/>
+    </row>
+    <row r="13">
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E12:F12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>